<commit_message>
add boyidol some question
</commit_message>
<xml_diff>
--- a/Questions/boyIdol.xlsx
+++ b/Questions/boyIdol.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jun/My Works/Rails/speedQuizRails/Questions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{167D949A-B6FB-8E42-88A6-2D9B081E7EE2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9470357-F376-234F-B3E9-656FEFC1FBA9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="500" windowWidth="28300" windowHeight="16940" xr2:uid="{B7182C66-C5DA-C947-81EE-F464D3AABB1E}"/>
+    <workbookView xWindow="240" yWindow="540" windowWidth="28300" windowHeight="16940" xr2:uid="{B7182C66-C5DA-C947-81EE-F464D3AABB1E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
   <si>
     <t>id</t>
   </si>
@@ -75,10 +75,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>방탄</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>비원에이포</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -87,10 +83,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>BIXX</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>엔시티</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -233,6 +225,42 @@
   <si>
     <t>MIB</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2GRP1rkE4O0</t>
+  </si>
+  <si>
+    <t>I3dezFzsNss</t>
+  </si>
+  <si>
+    <t>N8VRaGe3Cqs</t>
+  </si>
+  <si>
+    <t>Le0CwBy4SaQ</t>
+  </si>
+  <si>
+    <t>VIXX vixx</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ZAzWT8mRoR0</t>
+  </si>
+  <si>
+    <t>방탄소년단</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>gdZLi9oWNZg</t>
+  </si>
+  <si>
+    <t>방탄 BTS bts</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>sv53BwhUTC0</t>
+  </si>
+  <si>
+    <t>0IpbvXVbBYA</t>
   </si>
 </sst>
 </file>
@@ -608,7 +636,7 @@
   <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -634,6 +662,12 @@
       <c r="A2">
         <v>1</v>
       </c>
+      <c r="B2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2">
+        <v>13</v>
+      </c>
       <c r="D2" t="s">
         <v>5</v>
       </c>
@@ -642,6 +676,12 @@
       <c r="A3">
         <v>2</v>
       </c>
+      <c r="B3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
       <c r="D3" t="s">
         <v>6</v>
       </c>
@@ -653,6 +693,12 @@
       <c r="A4">
         <v>3</v>
       </c>
+      <c r="B4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4">
+        <v>77</v>
+      </c>
       <c r="D4" t="s">
         <v>8</v>
       </c>
@@ -661,6 +707,12 @@
       <c r="A5">
         <v>4</v>
       </c>
+      <c r="B5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5">
+        <v>80</v>
+      </c>
       <c r="D5" t="s">
         <v>9</v>
       </c>
@@ -669,41 +721,68 @@
       <c r="A6">
         <v>5</v>
       </c>
+      <c r="B6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6">
+        <v>57</v>
+      </c>
       <c r="D6" t="s">
         <v>10</v>
       </c>
       <c r="E6" t="s">
-        <v>14</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7">
         <v>6</v>
       </c>
+      <c r="B7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7">
+        <v>23</v>
+      </c>
       <c r="D7" t="s">
-        <v>11</v>
+        <v>55</v>
+      </c>
+      <c r="E7" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8">
         <v>7</v>
       </c>
+      <c r="B8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8">
+        <v>60</v>
+      </c>
       <c r="D8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" t="s">
         <v>12</v>
-      </c>
-      <c r="E8" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9">
         <v>8</v>
       </c>
+      <c r="B9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C9">
+        <v>57</v>
+      </c>
       <c r="D9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -711,7 +790,7 @@
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -719,7 +798,7 @@
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -727,7 +806,7 @@
         <v>11</v>
       </c>
       <c r="D12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -735,7 +814,7 @@
         <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -743,7 +822,7 @@
         <v>13</v>
       </c>
       <c r="D14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -751,7 +830,7 @@
         <v>14</v>
       </c>
       <c r="D15" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -759,7 +838,7 @@
         <v>15</v>
       </c>
       <c r="D16" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -767,10 +846,10 @@
         <v>16</v>
       </c>
       <c r="D17" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E17" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -778,10 +857,10 @@
         <v>17</v>
       </c>
       <c r="D18" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E18" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -789,10 +868,10 @@
         <v>18</v>
       </c>
       <c r="D19" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E19" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -800,10 +879,10 @@
         <v>19</v>
       </c>
       <c r="D20" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E20" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -811,10 +890,10 @@
         <v>20</v>
       </c>
       <c r="D21" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E21" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -822,10 +901,10 @@
         <v>21</v>
       </c>
       <c r="D22" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E22" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -833,7 +912,7 @@
         <v>22</v>
       </c>
       <c r="D23" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -841,7 +920,7 @@
         <v>23</v>
       </c>
       <c r="D24" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -849,7 +928,7 @@
         <v>24</v>
       </c>
       <c r="D25" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -857,10 +936,10 @@
         <v>25</v>
       </c>
       <c r="D26" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -868,10 +947,10 @@
         <v>26</v>
       </c>
       <c r="D27" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E27" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -879,7 +958,7 @@
         <v>27</v>
       </c>
       <c r="D28" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -887,7 +966,7 @@
         <v>28</v>
       </c>
       <c r="D29" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -895,10 +974,10 @@
         <v>29</v>
       </c>
       <c r="D30" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E30" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -906,10 +985,10 @@
         <v>30</v>
       </c>
       <c r="D31" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E31" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -917,7 +996,7 @@
         <v>31</v>
       </c>
       <c r="D32" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -925,7 +1004,7 @@
         <v>32</v>
       </c>
       <c r="D33" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>